<commit_message>
checklist and added to cleaning.
</commit_message>
<xml_diff>
--- a/data/raw/EDA Summary.xlsx
+++ b/data/raw/EDA Summary.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christine\Desktop\IT476\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\teradata\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F4CDC6-3D46-498F-AECE-2AE93E526A61}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8C9F05-98DD-4452-9854-A99A1BB97741}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48420" yWindow="30" windowWidth="17280" windowHeight="8970" xr2:uid="{DF3F421E-1078-4E2D-8514-4BCF3A33D0AB}"/>
+    <workbookView xWindow="9150" yWindow="990" windowWidth="19605" windowHeight="11175" xr2:uid="{DF3F421E-1078-4E2D-8514-4BCF3A33D0AB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data Type Setting" sheetId="1" r:id="rId1"/>
+    <sheet name="Deeper Clean" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="143">
   <si>
     <t>Campaign</t>
   </si>
@@ -400,6 +401,60 @@
   </si>
   <si>
     <t>int to text</t>
+  </si>
+  <si>
+    <t>COMPLETE</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>OwnerID =  HH employe ID (I Think)</t>
+  </si>
+  <si>
+    <t>split into city and state cols</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Need</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Security_clearance_description__c</t>
+  </si>
+  <si>
+    <t>cut dates and replace with text</t>
+  </si>
+  <si>
+    <t>Languages_spoken__c</t>
+  </si>
+  <si>
+    <t>clean up and aggregate</t>
+  </si>
+  <si>
+    <t>Job_type__C</t>
+  </si>
+  <si>
+    <t>split and aggregate</t>
+  </si>
+  <si>
+    <t>Desired_state_of_employment__c</t>
+  </si>
+  <si>
+    <t>clean and aggreate</t>
+  </si>
+  <si>
+    <t>Min_salary_expected__c</t>
+  </si>
+  <si>
+    <t>normalize and split into hourly and annually</t>
   </si>
 </sst>
 </file>
@@ -415,15 +470,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -431,12 +492,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,25 +828,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F27F1DF-0459-4A7B-B0F0-42344871889B}">
-  <dimension ref="A1:H110"/>
+  <dimension ref="A1:J110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <pane ySplit="2" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I93" sqref="I93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>104</v>
       </c>
@@ -794,8 +875,14 @@
       <c r="H2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -805,8 +892,11 @@
       <c r="C3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -822,8 +912,11 @@
       <c r="F4" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -833,8 +926,11 @@
       <c r="C5" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -844,8 +940,11 @@
       <c r="C6" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -855,8 +954,14 @@
       <c r="C7" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>116</v>
+      </c>
+      <c r="I7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -866,8 +971,11 @@
       <c r="C8" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -877,8 +985,11 @@
       <c r="C9" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -891,8 +1002,11 @@
       <c r="E10" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -905,8 +1019,11 @@
       <c r="E11" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -916,8 +1033,11 @@
       <c r="C12" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -930,8 +1050,11 @@
       <c r="F13" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -941,8 +1064,14 @@
       <c r="C14" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -952,8 +1081,14 @@
       <c r="C15" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>116</v>
+      </c>
+      <c r="I15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -963,8 +1098,11 @@
       <c r="C16" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -977,8 +1115,11 @@
       <c r="D17" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -988,8 +1129,11 @@
       <c r="C18" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -999,8 +1143,11 @@
       <c r="C19" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1010,8 +1157,11 @@
       <c r="C20" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1021,8 +1171,11 @@
       <c r="C21" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1032,8 +1185,11 @@
       <c r="C22" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1043,8 +1199,11 @@
       <c r="C23" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1054,8 +1213,11 @@
       <c r="C24" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I24" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1065,8 +1227,11 @@
       <c r="C25" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1076,8 +1241,11 @@
       <c r="C26" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1087,8 +1255,11 @@
       <c r="C27" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1098,8 +1269,11 @@
       <c r="C28" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1109,8 +1283,11 @@
       <c r="C29" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -1120,8 +1297,11 @@
       <c r="C30" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -1131,8 +1311,11 @@
       <c r="C31" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I31" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -1142,8 +1325,11 @@
       <c r="C32" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -1153,8 +1339,11 @@
       <c r="C33" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I33" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -1164,8 +1353,11 @@
       <c r="C34" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I34" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -1175,8 +1367,11 @@
       <c r="C35" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I35" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -1186,8 +1381,11 @@
       <c r="C36" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -1197,8 +1395,11 @@
       <c r="C37" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I37" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -1208,8 +1409,11 @@
       <c r="C38" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I38" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>0</v>
       </c>
@@ -1222,8 +1426,14 @@
       <c r="G39" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I39" t="s">
+        <v>116</v>
+      </c>
+      <c r="J39" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -1236,8 +1446,11 @@
       <c r="E40" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I40" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -1247,8 +1460,11 @@
       <c r="C41" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -1261,8 +1477,11 @@
       <c r="E42" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I42" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -1275,8 +1494,11 @@
       <c r="G43" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I43" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>0</v>
       </c>
@@ -1289,8 +1511,11 @@
       <c r="E44" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I44" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -1303,8 +1528,11 @@
       <c r="E45" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -1317,8 +1545,11 @@
       <c r="F46" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I46" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>0</v>
       </c>
@@ -1328,8 +1559,11 @@
       <c r="C47" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I47" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>0</v>
       </c>
@@ -1339,8 +1573,11 @@
       <c r="C48" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I48" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -1350,8 +1587,11 @@
       <c r="C49" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I49" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -1361,8 +1601,11 @@
       <c r="C50" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I50" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>0</v>
       </c>
@@ -1372,8 +1615,11 @@
       <c r="C51" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I51" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>0</v>
       </c>
@@ -1386,8 +1632,11 @@
       <c r="F52" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I52" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -1397,8 +1646,11 @@
       <c r="C53" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I53" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>0</v>
       </c>
@@ -1411,8 +1663,11 @@
       <c r="D54" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I54" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>0</v>
       </c>
@@ -1422,8 +1677,14 @@
       <c r="C55" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D55" t="s">
+        <v>116</v>
+      </c>
+      <c r="I55" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>0</v>
       </c>
@@ -1433,8 +1694,14 @@
       <c r="C56" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I56" t="s">
+        <v>116</v>
+      </c>
+      <c r="J56" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -1447,8 +1714,11 @@
       <c r="D57" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I57" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>0</v>
       </c>
@@ -1461,8 +1731,11 @@
       <c r="F58" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I58" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>0</v>
       </c>
@@ -1475,8 +1748,11 @@
       <c r="F59" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I59" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>0</v>
       </c>
@@ -1486,8 +1762,11 @@
       <c r="C60" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I60" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>0</v>
       </c>
@@ -1497,8 +1776,11 @@
       <c r="C61" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I61" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -1511,8 +1793,11 @@
       <c r="F62" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I62" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>0</v>
       </c>
@@ -1522,8 +1807,11 @@
       <c r="C63" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I63" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>0</v>
       </c>
@@ -1536,8 +1824,11 @@
       <c r="D64" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I64" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>0</v>
       </c>
@@ -1550,8 +1841,11 @@
       <c r="G65" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I65" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>0</v>
       </c>
@@ -1564,8 +1858,11 @@
       <c r="G66" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I66" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -1578,8 +1875,11 @@
       <c r="G67" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I67" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>0</v>
       </c>
@@ -1589,8 +1889,14 @@
       <c r="C68" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D68" t="s">
+        <v>116</v>
+      </c>
+      <c r="I68" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>0</v>
       </c>
@@ -1600,8 +1906,11 @@
       <c r="C69" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I69" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>0</v>
       </c>
@@ -1614,8 +1923,11 @@
       <c r="H70" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I70" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>0</v>
       </c>
@@ -1625,8 +1937,11 @@
       <c r="C71" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I71" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>0</v>
       </c>
@@ -1636,8 +1951,11 @@
       <c r="C72" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I72" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>0</v>
       </c>
@@ -1653,8 +1971,11 @@
       <c r="H73" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I73" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>0</v>
       </c>
@@ -1667,8 +1988,11 @@
       <c r="H74" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I74" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>0</v>
       </c>
@@ -1681,8 +2005,11 @@
       <c r="H75" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I75" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>0</v>
       </c>
@@ -1695,8 +2022,11 @@
       <c r="F76" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I76" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>0</v>
       </c>
@@ -1712,8 +2042,11 @@
       <c r="H77" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I77" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>0</v>
       </c>
@@ -1729,8 +2062,11 @@
       <c r="H78" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I78" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>0</v>
       </c>
@@ -1746,8 +2082,11 @@
       <c r="H79" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I79" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>0</v>
       </c>
@@ -1760,8 +2099,11 @@
       <c r="G80" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I80" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>0</v>
       </c>
@@ -1771,8 +2113,14 @@
       <c r="C81" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H81" t="s">
+        <v>116</v>
+      </c>
+      <c r="I81" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>0</v>
       </c>
@@ -1785,8 +2133,11 @@
       <c r="D82" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I82" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>0</v>
       </c>
@@ -1796,8 +2147,14 @@
       <c r="C83" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E83" t="s">
+        <v>116</v>
+      </c>
+      <c r="I83" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>0</v>
       </c>
@@ -1810,24 +2167,45 @@
       <c r="F84" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I84" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>0</v>
       </c>
       <c r="B85" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C85" t="s">
+        <v>113</v>
+      </c>
+      <c r="E85" t="s">
+        <v>116</v>
+      </c>
+      <c r="I85" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>0</v>
       </c>
       <c r="B86" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C86" t="s">
+        <v>113</v>
+      </c>
+      <c r="D86" t="s">
+        <v>116</v>
+      </c>
+      <c r="I86" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>0</v>
       </c>
@@ -1835,7 +2213,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>0</v>
       </c>
@@ -1843,7 +2221,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>0</v>
       </c>
@@ -1851,7 +2229,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>0</v>
       </c>
@@ -1859,7 +2237,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>0</v>
       </c>
@@ -1867,7 +2245,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>0</v>
       </c>
@@ -1875,7 +2253,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>0</v>
       </c>
@@ -1883,7 +2261,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>0</v>
       </c>
@@ -1891,7 +2269,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>0</v>
       </c>
@@ -1899,7 +2277,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>0</v>
       </c>
@@ -1907,7 +2285,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>0</v>
       </c>
@@ -1915,7 +2293,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>0</v>
       </c>
@@ -1923,7 +2301,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>0</v>
       </c>
@@ -1931,7 +2309,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>0</v>
       </c>
@@ -1939,7 +2317,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>0</v>
       </c>
@@ -1950,7 +2328,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>0</v>
       </c>
@@ -1958,7 +2336,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>0</v>
       </c>
@@ -1966,7 +2344,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>0</v>
       </c>
@@ -1974,7 +2352,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>0</v>
       </c>
@@ -1982,7 +2360,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>112</v>
       </c>
@@ -1990,7 +2368,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>112</v>
       </c>
@@ -1998,7 +2376,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>112</v>
       </c>
@@ -2006,7 +2384,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>112</v>
       </c>
@@ -2014,7 +2392,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>112</v>
       </c>
@@ -2026,4 +2404,89 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56AD02D9-1688-45E1-8643-7F7CBD2ED4AB}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="3" width="39.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
clean languages in contacts df.
</commit_message>
<xml_diff>
--- a/data/raw/EDA Summary.xlsx
+++ b/data/raw/EDA Summary.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\teradata\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8C9F05-98DD-4452-9854-A99A1BB97741}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D039D18-2FFE-4E38-9578-9623A2392409}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9150" yWindow="990" windowWidth="19605" windowHeight="11175" xr2:uid="{DF3F421E-1078-4E2D-8514-4BCF3A33D0AB}"/>
+    <workbookView xWindow="8400" yWindow="990" windowWidth="19605" windowHeight="11175" activeTab="1" xr2:uid="{DF3F421E-1078-4E2D-8514-4BCF3A33D0AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Type Setting" sheetId="1" r:id="rId1"/>
-    <sheet name="Deeper Clean" sheetId="2" r:id="rId2"/>
+    <sheet name="Deeper Cleaning needs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -830,7 +830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F27F1DF-0459-4A7B-B0F0-42344871889B}">
   <dimension ref="A1:J110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I93" sqref="I93"/>
     </sheetView>
@@ -2410,8 +2410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56AD02D9-1688-45E1-8643-7F7CBD2ED4AB}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
clean states and slaray expectations in contacts, update checklist.
</commit_message>
<xml_diff>
--- a/data/raw/EDA Summary.xlsx
+++ b/data/raw/EDA Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\teradata\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D039D18-2FFE-4E38-9578-9623A2392409}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C2CCA4-FB72-437F-AE54-5DC908FDFB17}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8400" yWindow="990" windowWidth="19605" windowHeight="11175" activeTab="1" xr2:uid="{DF3F421E-1078-4E2D-8514-4BCF3A33D0AB}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="146">
   <si>
     <t>Campaign</t>
   </si>
@@ -455,6 +455,15 @@
   </si>
   <si>
     <t>normalize and split into hourly and annually</t>
+  </si>
+  <si>
+    <t>COMPLETION NOTES</t>
+  </si>
+  <si>
+    <t>split into new variables</t>
+  </si>
+  <si>
+    <t>split into type, annual, and hourly variables</t>
   </si>
 </sst>
 </file>
@@ -484,7 +493,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -507,13 +516,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2408,19 +2429,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56AD02D9-1688-45E1-8643-7F7CBD2ED4AB}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33.85546875" customWidth="1"/>
     <col min="3" max="3" width="39.5703125" customWidth="1"/>
+    <col min="5" max="5" width="43.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>129</v>
       </c>
@@ -2430,8 +2452,14 @@
       <c r="C1" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>132</v>
       </c>
@@ -2441,8 +2469,11 @@
       <c r="C2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>132</v>
       </c>
@@ -2452,8 +2483,11 @@
       <c r="C3" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>132</v>
       </c>
@@ -2463,8 +2497,14 @@
       <c r="C4" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>132</v>
       </c>
@@ -2474,8 +2514,11 @@
       <c r="C5" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>132</v>
       </c>
@@ -2484,6 +2527,12 @@
       </c>
       <c r="C6" t="s">
         <v>142</v>
+      </c>
+      <c r="D6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>